<commit_message>
typos and errors in files
</commit_message>
<xml_diff>
--- a/data/microscopy/microscopy.xlsx
+++ b/data/microscopy/microscopy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GW-May" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="389">
   <si>
     <t xml:space="preserve">TUBE ID</t>
   </si>
@@ -1114,9 +1114,6 @@
   </si>
   <si>
     <t xml:space="preserve">WB628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SITE</t>
   </si>
   <si>
     <t xml:space="preserve">Corphium_sp.</t>
@@ -3946,7 +3943,7 @@
   </sheetPr>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -9082,8 +9079,8 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9109,7 +9106,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>363</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
@@ -9170,7 +9167,7 @@
         <v>335</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>7</v>
@@ -9204,7 +9201,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>43012</v>
@@ -9271,10 +9268,10 @@
         <v>103</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1</v>
@@ -9308,7 +9305,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>43012</v>
@@ -9334,7 +9331,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>43012</v>
@@ -9360,7 +9357,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>43012</v>
@@ -9386,7 +9383,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>43012</v>
@@ -9412,7 +9409,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>43012</v>
@@ -9438,25 +9435,25 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>43012</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="B14" s="4" t="n">
-        <v>43012</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>374</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>1</v>
@@ -9612,7 +9609,7 @@
         <v>42</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
@@ -9620,7 +9617,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>43012</v>
@@ -9646,7 +9643,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>43012</v>
@@ -9664,7 +9661,7 @@
         <v>42</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>1</v>
@@ -9947,7 +9944,7 @@
         <v>103</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>333</v>
@@ -9973,10 +9970,10 @@
         <v>103</v>
       </c>
       <c r="F34" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>380</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>1</v>
@@ -10010,7 +10007,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>43012</v>
@@ -10025,7 +10022,7 @@
         <v>82</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>308</v>
@@ -10036,7 +10033,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>43012</v>
@@ -10051,7 +10048,7 @@
         <v>82</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>245</v>
@@ -10132,7 +10129,7 @@
         <v>47</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>1</v>
@@ -10244,7 +10241,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B45" s="4" t="n">
         <v>43012</v>
@@ -10270,7 +10267,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B46" s="4" t="n">
         <v>43012</v>
@@ -10296,7 +10293,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B47" s="4" t="n">
         <v>43012</v>
@@ -10322,7 +10319,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B48" s="4" t="n">
         <v>43012</v>
@@ -10363,7 +10360,7 @@
         <v>82</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>308</v>
@@ -10392,7 +10389,7 @@
         <v>47</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>1</v>
@@ -10452,7 +10449,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B53" s="4" t="n">
         <v>43012</v>
@@ -10571,10 +10568,10 @@
         <v>32</v>
       </c>
       <c r="F57" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="G57" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>374</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>1</v>
@@ -10675,10 +10672,10 @@
         <v>32</v>
       </c>
       <c r="F61" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="G61" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>374</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
typos in microscopy plus cleaning of frames in main script
</commit_message>
<xml_diff>
--- a/data/microscopy/microscopy.xlsx
+++ b/data/microscopy/microscopy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GW-May" sheetId="1" state="visible" r:id="rId2"/>
@@ -1321,7 +1321,7 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6110,15 +6110,16 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.67"/>
@@ -6161,6 +6162,9 @@
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E2" s="0" t="s">
         <v>32</v>
       </c>
@@ -6184,6 +6188,9 @@
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E3" s="0" t="s">
         <v>32</v>
       </c>
@@ -6207,6 +6214,9 @@
       <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E4" s="0" t="s">
         <v>32</v>
       </c>
@@ -6230,6 +6240,9 @@
       <c r="C5" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E5" s="0" t="s">
         <v>10</v>
       </c>
@@ -6253,6 +6266,9 @@
       <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" s="0" t="s">
         <v>32</v>
       </c>
@@ -6276,6 +6292,9 @@
       <c r="C7" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E7" s="0" t="s">
         <v>103</v>
       </c>
@@ -6299,6 +6318,9 @@
       <c r="C8" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="0" t="s">
         <v>103</v>
       </c>
@@ -6322,6 +6344,9 @@
       <c r="C9" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="0" t="s">
         <v>103</v>
       </c>
@@ -6345,6 +6370,9 @@
       <c r="C10" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E10" s="0" t="s">
         <v>103</v>
       </c>
@@ -6368,6 +6396,9 @@
       <c r="C11" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E11" s="0" t="s">
         <v>32</v>
       </c>
@@ -6391,6 +6422,9 @@
       <c r="C12" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E12" s="0" t="s">
         <v>32</v>
       </c>
@@ -6414,6 +6448,9 @@
       <c r="C13" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E13" s="0" t="s">
         <v>82</v>
       </c>
@@ -6437,6 +6474,9 @@
       <c r="C14" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E14" s="0" t="s">
         <v>10</v>
       </c>
@@ -6460,6 +6500,9 @@
       <c r="C15" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E15" s="0" t="s">
         <v>103</v>
       </c>
@@ -6483,6 +6526,9 @@
       <c r="C16" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E16" s="0" t="s">
         <v>82</v>
       </c>
@@ -6506,6 +6552,9 @@
       <c r="C17" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E17" s="0" t="s">
         <v>82</v>
       </c>
@@ -6529,6 +6578,9 @@
       <c r="C18" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E18" s="0" t="s">
         <v>32</v>
       </c>
@@ -6552,6 +6604,9 @@
       <c r="C19" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E19" s="0" t="s">
         <v>32</v>
       </c>
@@ -6575,6 +6630,9 @@
       <c r="C20" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E20" s="0" t="s">
         <v>32</v>
       </c>
@@ -6598,6 +6656,9 @@
       <c r="C21" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E21" s="0" t="s">
         <v>32</v>
       </c>
@@ -6621,6 +6682,9 @@
       <c r="C22" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E22" s="0" t="s">
         <v>60</v>
       </c>
@@ -6644,6 +6708,9 @@
       <c r="C23" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="0" t="s">
         <v>198</v>
       </c>
@@ -6667,6 +6734,9 @@
       <c r="C24" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E24" s="0" t="s">
         <v>103</v>
       </c>
@@ -6690,6 +6760,9 @@
       <c r="C25" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E25" s="0" t="s">
         <v>103</v>
       </c>
@@ -6713,6 +6786,9 @@
       <c r="C26" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E26" s="0" t="s">
         <v>103</v>
       </c>
@@ -6736,6 +6812,9 @@
       <c r="C27" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E27" s="0" t="s">
         <v>103</v>
       </c>
@@ -6759,6 +6838,9 @@
       <c r="C28" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E28" s="0" t="s">
         <v>82</v>
       </c>
@@ -6782,6 +6864,9 @@
       <c r="C29" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E29" s="0" t="s">
         <v>60</v>
       </c>
@@ -6805,6 +6890,9 @@
       <c r="C30" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E30" s="0" t="s">
         <v>82</v>
       </c>
@@ -6828,6 +6916,9 @@
       <c r="C31" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E31" s="0" t="s">
         <v>10</v>
       </c>
@@ -6851,6 +6942,9 @@
       <c r="C32" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E32" s="0" t="s">
         <v>103</v>
       </c>
@@ -6874,6 +6968,9 @@
       <c r="C33" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E33" s="0" t="s">
         <v>32</v>
       </c>
@@ -6897,6 +6994,9 @@
       <c r="C34" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D34" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E34" s="0" t="s">
         <v>99</v>
       </c>
@@ -6920,6 +7020,9 @@
       <c r="C35" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D35" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E35" s="0" t="s">
         <v>103</v>
       </c>
@@ -6943,6 +7046,9 @@
       <c r="C36" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D36" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E36" s="0" t="s">
         <v>51</v>
       </c>
@@ -6966,6 +7072,9 @@
       <c r="C37" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D37" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E37" s="0" t="s">
         <v>10</v>
       </c>
@@ -6989,6 +7098,9 @@
       <c r="C38" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D38" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E38" s="0" t="s">
         <v>32</v>
       </c>
@@ -7012,6 +7124,9 @@
       <c r="C39" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D39" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E39" s="0" t="s">
         <v>103</v>
       </c>
@@ -7035,6 +7150,9 @@
       <c r="C40" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D40" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E40" s="0" t="s">
         <v>32</v>
       </c>
@@ -7058,6 +7176,9 @@
       <c r="C41" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D41" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E41" s="0" t="s">
         <v>23</v>
       </c>
@@ -7081,6 +7202,9 @@
       <c r="C42" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D42" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E42" s="0" t="s">
         <v>51</v>
       </c>
@@ -7104,6 +7228,9 @@
       <c r="C43" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D43" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E43" s="0" t="s">
         <v>32</v>
       </c>
@@ -7127,6 +7254,9 @@
       <c r="C44" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D44" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E44" s="0" t="s">
         <v>32</v>
       </c>
@@ -7150,6 +7280,9 @@
       <c r="C45" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D45" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E45" s="0" t="s">
         <v>32</v>
       </c>
@@ -7173,6 +7306,9 @@
       <c r="C46" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D46" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E46" s="0" t="s">
         <v>32</v>
       </c>
@@ -7196,6 +7332,9 @@
       <c r="C47" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D47" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E47" s="0" t="s">
         <v>132</v>
       </c>
@@ -7219,6 +7358,9 @@
       <c r="C48" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D48" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E48" s="0" t="s">
         <v>103</v>
       </c>
@@ -7242,6 +7384,9 @@
       <c r="C49" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D49" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E49" s="0" t="s">
         <v>103</v>
       </c>
@@ -7265,6 +7410,9 @@
       <c r="C50" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D50" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E50" s="0" t="s">
         <v>60</v>
       </c>
@@ -7288,6 +7436,9 @@
       <c r="C51" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D51" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="E51" s="0" t="s">
         <v>32</v>
       </c>
@@ -7311,6 +7462,9 @@
       <c r="C52" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D52" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="E52" s="0" t="s">
         <v>32</v>
       </c>
@@ -7334,6 +7488,9 @@
       <c r="C53" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D53" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="E53" s="0" t="s">
         <v>23</v>
       </c>
@@ -7357,6 +7514,9 @@
       <c r="C54" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D54" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="E54" s="0" t="s">
         <v>82</v>
       </c>
@@ -7380,6 +7540,9 @@
       <c r="C55" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="D55" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="E55" s="0" t="s">
         <v>103</v>
       </c>
@@ -7402,6 +7565,9 @@
       </c>
       <c r="C56" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>103</v>
@@ -9079,7 +9245,7 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>